<commit_message>
POL-3138: Stricter Hub finding (#2531)
* POL-3138: stricter hub finding

* POL-3138: stricter lookups mean changes to files

* POL-3138: fixed/removed specs

* POL-3138: skip v2 spec

* POL-3138: Prioritize Locode over Country due to country names

* POL-3138: added more specs
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_pricings_dynamic.xlsx
+++ b/spec/fixtures/files/excel/example_pricings_dynamic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>GROUP_ID</t>
   </si>
@@ -82,9 +82,21 @@
     <t>LSS</t>
   </si>
   <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Gothenburg</t>
+  </si>
+  <si>
     <t>SEGOT</t>
   </si>
   <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
     <t>CNSHA</t>
   </si>
   <si>
@@ -107,18 +119,6 @@
   </si>
   <si>
     <t>USD</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Gothenburg</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
   </si>
   <si>
     <t>FCL_40</t>
@@ -139,6 +139,7 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -171,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -192,6 +193,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
@@ -410,10 +417,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="7" width="18.71"/>
-    <col customWidth="1" min="8" max="10" width="25.29"/>
+    <col customWidth="1" min="5" max="7" width="16.38"/>
+    <col customWidth="1" min="8" max="10" width="22.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,42 +507,50 @@
       <c r="D2" s="6">
         <v>44561.0</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="G2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="K2" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
-      <c r="V2" s="7">
+      <c r="V2" s="9">
         <v>4330.0</v>
       </c>
       <c r="W2" s="4">
@@ -555,44 +570,48 @@
       <c r="D3" s="6">
         <v>44561.0</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="E3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="7">
+      <c r="V3" s="9">
         <v>4660.0</v>
       </c>
       <c r="W3" s="4">
@@ -612,48 +631,48 @@
       <c r="D4" s="6">
         <v>44561.0</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H4" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-      <c r="V4" s="7">
+      <c r="V4" s="9">
         <v>5330.0</v>
       </c>
       <c r="W4" s="4">

</xml_diff>